<commit_message>
add func for btn
</commit_message>
<xml_diff>
--- a/NDL6Staff.xlsx
+++ b/NDL6Staff.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vivog\AppData\Local\Programs\Python\Python310-32\Projects\LabStaff32\dist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\NDL6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F960336E-9E1B-4C6E-8F43-D0C10EF3B914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19C42B9-920E-46B6-97D7-34F8DB379BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="24120" windowHeight="13020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NDL6Staff" sheetId="1" r:id="rId1"/>
@@ -20,16 +20,7 @@
     <sheet name="GOI" sheetId="5" r:id="rId5"/>
     <sheet name="GNO" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -66,9 +57,6 @@
     <t>Андреев В.В.</t>
   </si>
   <si>
-    <t>ведущий инженер-исследователь</t>
-  </si>
-  <si>
     <t>ул. Вокзальная 49, кв.53</t>
   </si>
   <si>
@@ -120,9 +108,6 @@
     <t>Дубчак В.В.</t>
   </si>
   <si>
-    <t>инженер-исследователь I категории</t>
-  </si>
-  <si>
     <t>ул. Чайковского 38, кв.2</t>
   </si>
   <si>
@@ -132,9 +117,6 @@
     <t>Дяченко К.С.</t>
   </si>
   <si>
-    <t>инженер-исследователь II категории</t>
-  </si>
-  <si>
     <t>ул. Озерная 25, кв.15</t>
   </si>
   <si>
@@ -207,9 +189,6 @@
     <t>Обелец О.Л.</t>
   </si>
   <si>
-    <t>инженер-электроник I категории</t>
-  </si>
-  <si>
     <t>ул. Чайковского 38, кв.25</t>
   </si>
   <si>
@@ -285,9 +264,6 @@
     <t>Уздяев С.Н.</t>
   </si>
   <si>
-    <t>инженер-исследователь без категории</t>
-  </si>
-  <si>
     <t>ул. Казарского 5Б, кв.57</t>
   </si>
   <si>
@@ -595,6 +571,21 @@
   </si>
   <si>
     <t>18.12.1995</t>
+  </si>
+  <si>
+    <t>вед инженер-исследователь</t>
+  </si>
+  <si>
+    <t>инженер-исследователь I кат</t>
+  </si>
+  <si>
+    <t>инженер-исследователь II кат</t>
+  </si>
+  <si>
+    <t>инженер-электроник I кат</t>
+  </si>
+  <si>
+    <t>инженер-исследователь без кат</t>
   </si>
 </sst>
 </file>
@@ -1460,8 +1451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,22 +1506,22 @@
         <v>13495</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>182</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F2">
         <v>10</v>
       </c>
       <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J2" s="1"/>
     </row>
@@ -1539,28 +1530,28 @@
         <v>56189</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>8955</v>
       </c>
       <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>15</v>
       </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
       <c r="I3" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -1569,28 +1560,28 @@
         <v>56020</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>9550</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
         <v>18</v>
       </c>
-      <c r="H4" t="s">
-        <v>19</v>
-      </c>
       <c r="I4" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="J4" s="1"/>
     </row>
@@ -1599,28 +1590,28 @@
         <v>56006</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>9900</v>
       </c>
       <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>22</v>
       </c>
-      <c r="H5" t="s">
-        <v>23</v>
-      </c>
       <c r="I5" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="J5" s="1"/>
     </row>
@@ -1629,28 +1620,28 @@
         <v>81939</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6">
         <v>8430</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
         <v>25</v>
       </c>
-      <c r="H6" t="s">
-        <v>26</v>
-      </c>
       <c r="I6" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="J6" s="1"/>
     </row>
@@ -1659,28 +1650,28 @@
         <v>56016</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7">
         <v>13850</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>183</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F7">
         <v>40</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="J7" s="1"/>
     </row>
@@ -1689,28 +1680,28 @@
         <v>81953</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C8">
         <v>13070</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>184</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F8">
         <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J8" s="1"/>
     </row>
@@ -1719,28 +1710,28 @@
         <v>56146</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C9">
         <v>12210</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="J9" s="1"/>
     </row>
@@ -1749,28 +1740,28 @@
         <v>56177</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C10">
         <v>11620</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="J10" s="1"/>
     </row>
@@ -1779,28 +1770,28 @@
         <v>56007</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C11">
         <v>9900</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="J11" s="1"/>
     </row>
@@ -1809,28 +1800,28 @@
         <v>58003</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C12">
         <v>13135</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="J12" s="1"/>
     </row>
@@ -1839,28 +1830,28 @@
         <v>56135</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C13">
         <v>11845</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -1869,28 +1860,28 @@
         <v>81960</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C14">
         <v>12870</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="J14" s="1"/>
     </row>
@@ -1899,28 +1890,28 @@
         <v>56134</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C15">
         <v>9535</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F15">
         <v>0</v>
       </c>
       <c r="G15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" t="s">
         <v>52</v>
       </c>
-      <c r="H15" t="s">
-        <v>55</v>
-      </c>
       <c r="I15" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="J15" s="1"/>
     </row>
@@ -1929,28 +1920,28 @@
         <v>58016</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C16">
         <v>13795</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>185</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F16">
         <v>10</v>
       </c>
       <c r="G16" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H16" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="J16" s="1"/>
     </row>
@@ -1959,28 +1950,28 @@
         <v>56188</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C17">
         <v>8565</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="J17" s="1"/>
     </row>
@@ -1989,28 +1980,28 @@
         <v>81946</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C18">
         <v>11310</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H18" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="J18" s="1"/>
     </row>
@@ -2019,28 +2010,28 @@
         <v>56168</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C19">
         <v>9550</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="J19" s="1"/>
     </row>
@@ -2049,28 +2040,28 @@
         <v>81958</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C20">
         <v>19515</v>
       </c>
       <c r="D20" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="F20">
         <v>30</v>
       </c>
       <c r="G20" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H20" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="J20" s="1"/>
     </row>
@@ -2079,28 +2070,28 @@
         <v>81706</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C21">
         <v>10890</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H21" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -2109,28 +2100,28 @@
         <v>53165</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C22">
         <v>10330</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="F22">
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H22" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="J22" s="1"/>
     </row>
@@ -2139,28 +2130,28 @@
         <v>56012</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C23">
         <v>12305</v>
       </c>
       <c r="D23" t="s">
-        <v>28</v>
+        <v>183</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F23">
         <v>25</v>
       </c>
       <c r="G23" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H23" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="J23" s="1"/>
     </row>
@@ -2169,28 +2160,28 @@
         <v>56185</v>
       </c>
       <c r="B24" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C24">
         <v>12120</v>
       </c>
       <c r="D24" t="s">
-        <v>32</v>
+        <v>184</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F24">
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H24" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="J24" s="1"/>
     </row>
@@ -2199,28 +2190,28 @@
         <v>56136</v>
       </c>
       <c r="B25" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C25">
         <v>12100</v>
       </c>
       <c r="D25" t="s">
-        <v>28</v>
+        <v>183</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="F25">
         <v>15</v>
       </c>
       <c r="G25" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H25" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="J25" s="1"/>
     </row>
@@ -2229,28 +2220,28 @@
         <v>56169</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C26">
         <v>12555</v>
       </c>
       <c r="D26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="F26">
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H26" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="J26" s="1"/>
     </row>
@@ -2259,28 +2250,28 @@
         <v>56002</v>
       </c>
       <c r="B27" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C27">
         <v>15110</v>
       </c>
       <c r="D27" t="s">
-        <v>10</v>
+        <v>182</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F27">
         <v>40</v>
       </c>
       <c r="G27" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H27" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="J27" s="1"/>
     </row>
@@ -2289,28 +2280,28 @@
         <v>56145</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C28">
         <v>10890</v>
       </c>
       <c r="D28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="F28">
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H28" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="J28" s="1"/>
     </row>
@@ -2319,28 +2310,28 @@
         <v>81851</v>
       </c>
       <c r="B29" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C29">
         <v>11845</v>
       </c>
       <c r="D29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F29">
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H29" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="J29" s="1"/>
     </row>
@@ -2349,28 +2340,28 @@
         <v>56019</v>
       </c>
       <c r="B30" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C30">
         <v>11100</v>
       </c>
       <c r="D30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F30">
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="H30" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="J30" s="1"/>
     </row>
@@ -2379,28 +2370,28 @@
         <v>4073</v>
       </c>
       <c r="B31" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C31">
         <v>9550</v>
       </c>
       <c r="D31" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F31">
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H31" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="J31" s="1"/>
     </row>
@@ -2409,28 +2400,28 @@
         <v>56200</v>
       </c>
       <c r="B32" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C32">
         <v>9240</v>
       </c>
       <c r="D32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="F32">
         <v>0</v>
       </c>
       <c r="G32" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H32" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="J32" s="1"/>
     </row>
@@ -2439,28 +2430,28 @@
         <v>56201</v>
       </c>
       <c r="B33" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C33">
         <v>9240</v>
       </c>
       <c r="D33" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F33">
         <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H33" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="J33" s="1"/>
     </row>
@@ -2469,28 +2460,28 @@
         <v>56202</v>
       </c>
       <c r="B34" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C34">
         <v>9240</v>
       </c>
       <c r="D34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="F34">
         <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="H34" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="J34" s="1"/>
     </row>
@@ -2499,28 +2490,28 @@
         <v>56204</v>
       </c>
       <c r="B35" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C35">
         <v>9775</v>
       </c>
       <c r="D35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="F35">
         <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H35" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="J35" s="1"/>
     </row>
@@ -2529,28 +2520,28 @@
         <v>56205</v>
       </c>
       <c r="B36" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C36">
         <v>11000</v>
       </c>
       <c r="D36" t="s">
-        <v>83</v>
+        <v>186</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="F36">
         <v>0</v>
       </c>
       <c r="G36" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="H36" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2617,7 +2608,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2673,7 +2664,7 @@
       </c>
       <c r="D2" t="str">
         <f>NDL6Staff!D2</f>
-        <v>ведущий инженер-исследователь</v>
+        <v>вед инженер-исследователь</v>
       </c>
       <c r="E2" t="str">
         <f>NDL6Staff!E2</f>
@@ -3125,8 +3116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5C7ED1-4AFD-45F9-A987-03417CD707F2}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3255,7 +3246,7 @@
       </c>
       <c r="D4" t="str">
         <f>NDL6Staff!D23</f>
-        <v>инженер-исследователь I категории</v>
+        <v>инженер-исследователь I кат</v>
       </c>
       <c r="E4" t="str">
         <f>NDL6Staff!E23</f>
@@ -3370,7 +3361,7 @@
       </c>
       <c r="D7" t="str">
         <f>NDL6Staff!D36</f>
-        <v>инженер-исследователь без категории</v>
+        <v>инженер-исследователь без кат</v>
       </c>
       <c r="E7" t="str">
         <f>NDL6Staff!E36</f>
@@ -3457,7 +3448,7 @@
       </c>
       <c r="D2" t="str">
         <f>NDL6Staff!D8</f>
-        <v>инженер-исследователь II категории</v>
+        <v>инженер-исследователь II кат</v>
       </c>
       <c r="E2" t="str">
         <f>NDL6Staff!E8</f>
@@ -3571,7 +3562,7 @@
       </c>
       <c r="D5" t="str">
         <f>NDL6Staff!D24</f>
-        <v>инженер-исследователь II категории</v>
+        <v>инженер-исследователь II кат</v>
       </c>
       <c r="E5" t="str">
         <f>NDL6Staff!E24</f>
@@ -3850,7 +3841,7 @@
       </c>
       <c r="D2" t="str">
         <f>NDL6Staff!D7</f>
-        <v>инженер-исследователь I категории</v>
+        <v>инженер-исследователь I кат</v>
       </c>
       <c r="E2" t="str">
         <f>NDL6Staff!E7</f>
@@ -3888,7 +3879,7 @@
       </c>
       <c r="D3" t="str">
         <f>NDL6Staff!D25</f>
-        <v>инженер-исследователь I категории</v>
+        <v>инженер-исследователь I кат</v>
       </c>
       <c r="E3" t="str">
         <f>NDL6Staff!E25</f>
@@ -3926,7 +3917,7 @@
       </c>
       <c r="D4" t="str">
         <f>NDL6Staff!D27</f>
-        <v>ведущий инженер-исследователь</v>
+        <v>вед инженер-исследователь</v>
       </c>
       <c r="E4" t="str">
         <f>NDL6Staff!E27</f>
@@ -4051,7 +4042,7 @@
       </c>
       <c r="D3" t="str">
         <f>NDL6Staff!D16</f>
-        <v>инженер-электроник I категории</v>
+        <v>инженер-электроник I кат</v>
       </c>
       <c r="E3" t="str">
         <f>NDL6Staff!E16</f>

</xml_diff>